<commit_message>
(JS8) Tugas 1-3 KATEGORI
</commit_message>
<xml_diff>
--- a/public/template_level.xlsx
+++ b/public/template_level.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel putri\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F58894A-DD2D-47F5-ABDB-106E8A104E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2C1C76-4365-4CEA-94C3-FD435092116E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12780" yWindow="1290" windowWidth="6585" windowHeight="7785" xr2:uid="{D09AD215-BC86-4372-8DB0-02BCDD1DE2F9}"/>
+    <workbookView xWindow="13815" yWindow="2325" windowWidth="6585" windowHeight="7785" xr2:uid="{D09AD215-BC86-4372-8DB0-02BCDD1DE2F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>level_kode</t>
   </si>
@@ -33,16 +33,10 @@
     <t>level_nama</t>
   </si>
   <si>
-    <t>fitria</t>
+    <t>DIREKTUR</t>
   </si>
   <si>
     <t>syafa</t>
-  </si>
-  <si>
-    <t>STF</t>
-  </si>
-  <si>
-    <t>hertin</t>
   </si>
 </sst>
 </file>
@@ -394,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91EC98B1-BB63-4991-9AD2-D5CD08BDE7D3}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,26 +410,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>